<commit_message>
ai_pattern & snopes crawler
algorithm update:
1) find ai patterns for all pairwise of AC
2) Write the summary into csv

snopes.com crawler
1) crawl key information for fact-check source (source==1)
</commit_message>
<xml_diff>
--- a/apriori/aidata.xlsx
+++ b/apriori/aidata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agathos/DtotheS/AI-in-the-wild/apriori/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBFBAEF-7E91-0141-A920-1654F55FFD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8C6BFE-288C-2C4D-9382-0CCB0F904278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2020" windowWidth="28040" windowHeight="17440" xr2:uid="{887DE8EF-5DF0-C34D-A900-46871DFFD3F2}"/>
+    <workbookView xWindow="5620" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{887DE8EF-5DF0-C34D-A900-46871DFFD3F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="161">
   <si>
     <t>id</t>
   </si>
@@ -1406,6 +1407,27 @@
   <si>
     <t>mixed?</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>num_Bs</t>
+  </si>
+  <si>
+    <t>exist</t>
+  </si>
+  <si>
+    <t>non-exist</t>
+  </si>
+  <si>
+    <t>meaningful</t>
+  </si>
+  <si>
+    <t>unmeaningful</t>
+  </si>
 </sst>
 </file>
 
@@ -1414,7 +1436,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1818,11 +1840,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B5F6B6-0122-7C45-9BD1-C90B3603BC52}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I24" workbookViewId="0">
+    <sheetView topLeftCell="I24" workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
@@ -1835,7 +1857,7 @@
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +1886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1893,7 +1915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1922,7 +1944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1951,7 +1973,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1980,7 +2002,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -2009,7 +2031,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -2038,7 +2060,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -2067,7 +2089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -2096,7 +2118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -2125,7 +2147,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -2154,7 +2176,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -2183,7 +2205,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -2212,7 +2234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -2238,7 +2260,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -2264,7 +2286,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -2290,7 +2312,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -2316,7 +2338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -2342,7 +2364,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1">
+    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>3</v>
       </c>
@@ -2368,7 +2390,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -2397,7 +2419,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -2423,7 +2445,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -2452,7 +2474,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -2481,7 +2503,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -2507,7 +2529,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>4</v>
       </c>
@@ -2533,7 +2555,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -2559,7 +2581,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>4</v>
       </c>
@@ -2585,7 +2607,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -2611,7 +2633,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -2637,7 +2659,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -2663,7 +2685,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
@@ -2692,7 +2714,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>5</v>
       </c>
@@ -2718,7 +2740,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>5</v>
       </c>
@@ -2744,7 +2766,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>6</v>
       </c>
@@ -2773,7 +2795,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>6</v>
       </c>
@@ -2799,7 +2821,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>6</v>
       </c>
@@ -2825,7 +2847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>6</v>
       </c>
@@ -2851,13 +2873,13 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
     </row>
   </sheetData>
@@ -2885,4 +2907,45 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4020A137-8E4F-EA4D-AB19-D54723A17149}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>